<commit_message>
Actualizar las fechas de las tareas terminadas
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt STEPH Y HENRY.xlsx
+++ b/Diagrama de Gantt STEPH Y HENRY.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -1056,7 +1056,7 @@
     <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1189,9 +1189,6 @@
     <xf numFmtId="168" fontId="8" fillId="39" borderId="17" xfId="10" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="17" xfId="11" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="39" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1267,12 +1264,6 @@
     <xf numFmtId="0" fontId="32" fillId="44" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1284,6 +1275,12 @@
     </xf>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1344,18 +1341,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7"/>
@@ -1380,6 +1365,18 @@
         </left>
         <right style="thin">
           <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
         </right>
         <vertical/>
         <horizontal/>
@@ -1908,10 +1905,10 @@
   <dimension ref="A1:DW41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="7" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="7" topLeftCell="BQ20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1943,7 +1940,9 @@
     <col min="71" max="71" width="7.7109375" customWidth="1"/>
     <col min="72" max="77" width="3.28515625" customWidth="1"/>
     <col min="78" max="78" width="6" customWidth="1"/>
-    <col min="79" max="91" width="3.28515625" customWidth="1"/>
+    <col min="79" max="84" width="3.28515625" customWidth="1"/>
+    <col min="85" max="85" width="8" customWidth="1"/>
+    <col min="86" max="91" width="3.28515625" customWidth="1"/>
     <col min="92" max="92" width="5.140625" customWidth="1"/>
     <col min="93" max="98" width="3.28515625" customWidth="1"/>
     <col min="99" max="99" width="4.85546875" customWidth="1"/>
@@ -1977,203 +1976,203 @@
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="81">
+      <c r="D3" s="80"/>
+      <c r="E3" s="78">
         <v>45545</v>
       </c>
-      <c r="F3" s="81"/>
+      <c r="F3" s="78"/>
       <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="77"/>
+      <c r="D4" s="80"/>
       <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="I4" s="78">
+      <c r="I4" s="75">
         <f>I5</f>
         <v>45544</v>
       </c>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="78">
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="75">
         <f>P5</f>
         <v>45551</v>
       </c>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="79"/>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="78">
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="75">
         <f>W5</f>
         <v>45558</v>
       </c>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="79"/>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="78">
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="77"/>
+      <c r="AD4" s="75">
         <f>AD5</f>
         <v>45565</v>
       </c>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="79"/>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="80"/>
-      <c r="AK4" s="78">
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="77"/>
+      <c r="AK4" s="75">
         <f>AK5</f>
         <v>45572</v>
       </c>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="79"/>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="80"/>
-      <c r="AR4" s="78">
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="76"/>
+      <c r="AN4" s="76"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="77"/>
+      <c r="AR4" s="75">
         <f>AR5</f>
         <v>45579</v>
       </c>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="79"/>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="80"/>
-      <c r="AY4" s="78">
+      <c r="AS4" s="76"/>
+      <c r="AT4" s="76"/>
+      <c r="AU4" s="76"/>
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="76"/>
+      <c r="AX4" s="77"/>
+      <c r="AY4" s="75">
         <f>AY5</f>
         <v>45586</v>
       </c>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="79"/>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="78">
+      <c r="AZ4" s="76"/>
+      <c r="BA4" s="76"/>
+      <c r="BB4" s="76"/>
+      <c r="BC4" s="76"/>
+      <c r="BD4" s="76"/>
+      <c r="BE4" s="77"/>
+      <c r="BF4" s="75">
         <f>BF5</f>
         <v>45593</v>
       </c>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="79"/>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="80"/>
-      <c r="BM4" s="78">
+      <c r="BG4" s="76"/>
+      <c r="BH4" s="76"/>
+      <c r="BI4" s="76"/>
+      <c r="BJ4" s="76"/>
+      <c r="BK4" s="76"/>
+      <c r="BL4" s="77"/>
+      <c r="BM4" s="75">
         <f>BM5</f>
         <v>45600</v>
       </c>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="79"/>
-      <c r="BP4" s="79"/>
-      <c r="BQ4" s="79"/>
-      <c r="BR4" s="79"/>
-      <c r="BS4" s="80"/>
-      <c r="BT4" s="78">
+      <c r="BN4" s="76"/>
+      <c r="BO4" s="76"/>
+      <c r="BP4" s="76"/>
+      <c r="BQ4" s="76"/>
+      <c r="BR4" s="76"/>
+      <c r="BS4" s="77"/>
+      <c r="BT4" s="75">
         <f>BT5</f>
         <v>45607</v>
       </c>
-      <c r="BU4" s="79"/>
-      <c r="BV4" s="79"/>
-      <c r="BW4" s="79"/>
-      <c r="BX4" s="79"/>
-      <c r="BY4" s="79"/>
-      <c r="BZ4" s="80"/>
-      <c r="CA4" s="78">
+      <c r="BU4" s="76"/>
+      <c r="BV4" s="76"/>
+      <c r="BW4" s="76"/>
+      <c r="BX4" s="76"/>
+      <c r="BY4" s="76"/>
+      <c r="BZ4" s="77"/>
+      <c r="CA4" s="75">
         <f t="shared" ref="CA4" si="0">CA5</f>
         <v>45614</v>
       </c>
-      <c r="CB4" s="79"/>
-      <c r="CC4" s="79"/>
-      <c r="CD4" s="79"/>
-      <c r="CE4" s="79"/>
-      <c r="CF4" s="79"/>
-      <c r="CG4" s="80"/>
-      <c r="CH4" s="78">
+      <c r="CB4" s="76"/>
+      <c r="CC4" s="76"/>
+      <c r="CD4" s="76"/>
+      <c r="CE4" s="76"/>
+      <c r="CF4" s="76"/>
+      <c r="CG4" s="77"/>
+      <c r="CH4" s="75">
         <f t="shared" ref="CH4" si="1">CH5</f>
         <v>45621</v>
       </c>
-      <c r="CI4" s="79"/>
-      <c r="CJ4" s="79"/>
-      <c r="CK4" s="79"/>
-      <c r="CL4" s="79"/>
-      <c r="CM4" s="79"/>
-      <c r="CN4" s="80"/>
-      <c r="CO4" s="78">
+      <c r="CI4" s="76"/>
+      <c r="CJ4" s="76"/>
+      <c r="CK4" s="76"/>
+      <c r="CL4" s="76"/>
+      <c r="CM4" s="76"/>
+      <c r="CN4" s="77"/>
+      <c r="CO4" s="75">
         <f t="shared" ref="CO4" si="2">CO5</f>
         <v>45628</v>
       </c>
-      <c r="CP4" s="79"/>
-      <c r="CQ4" s="79"/>
-      <c r="CR4" s="79"/>
-      <c r="CS4" s="79"/>
-      <c r="CT4" s="79"/>
-      <c r="CU4" s="80"/>
-      <c r="CV4" s="78">
+      <c r="CP4" s="76"/>
+      <c r="CQ4" s="76"/>
+      <c r="CR4" s="76"/>
+      <c r="CS4" s="76"/>
+      <c r="CT4" s="76"/>
+      <c r="CU4" s="77"/>
+      <c r="CV4" s="75">
         <f t="shared" ref="CV4" si="3">CV5</f>
         <v>45635</v>
       </c>
-      <c r="CW4" s="79"/>
-      <c r="CX4" s="79"/>
-      <c r="CY4" s="79"/>
-      <c r="CZ4" s="79"/>
-      <c r="DA4" s="79"/>
-      <c r="DB4" s="80"/>
-      <c r="DC4" s="78">
+      <c r="CW4" s="76"/>
+      <c r="CX4" s="76"/>
+      <c r="CY4" s="76"/>
+      <c r="CZ4" s="76"/>
+      <c r="DA4" s="76"/>
+      <c r="DB4" s="77"/>
+      <c r="DC4" s="75">
         <f t="shared" ref="DC4" si="4">DC5</f>
         <v>45642</v>
       </c>
-      <c r="DD4" s="79"/>
-      <c r="DE4" s="79"/>
-      <c r="DF4" s="79"/>
-      <c r="DG4" s="79"/>
-      <c r="DH4" s="79"/>
-      <c r="DI4" s="80"/>
-      <c r="DJ4" s="78">
+      <c r="DD4" s="76"/>
+      <c r="DE4" s="76"/>
+      <c r="DF4" s="76"/>
+      <c r="DG4" s="76"/>
+      <c r="DH4" s="76"/>
+      <c r="DI4" s="77"/>
+      <c r="DJ4" s="75">
         <f t="shared" ref="DJ4" si="5">DJ5</f>
         <v>45649</v>
       </c>
-      <c r="DK4" s="79"/>
-      <c r="DL4" s="79"/>
-      <c r="DM4" s="79"/>
-      <c r="DN4" s="79"/>
-      <c r="DO4" s="79"/>
-      <c r="DP4" s="80"/>
-      <c r="DQ4" s="78">
+      <c r="DK4" s="76"/>
+      <c r="DL4" s="76"/>
+      <c r="DM4" s="76"/>
+      <c r="DN4" s="76"/>
+      <c r="DO4" s="76"/>
+      <c r="DP4" s="77"/>
+      <c r="DQ4" s="75">
         <f t="shared" ref="DQ4" si="6">DQ5</f>
         <v>45656</v>
       </c>
-      <c r="DR4" s="79"/>
-      <c r="DS4" s="79"/>
-      <c r="DT4" s="79"/>
-      <c r="DU4" s="79"/>
-      <c r="DV4" s="79"/>
-      <c r="DW4" s="80"/>
+      <c r="DR4" s="76"/>
+      <c r="DS4" s="76"/>
+      <c r="DT4" s="76"/>
+      <c r="DU4" s="76"/>
+      <c r="DV4" s="76"/>
+      <c r="DW4" s="77"/>
     </row>
     <row r="5" spans="1:127" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
@@ -3430,7 +3429,7 @@
     </row>
     <row r="9" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="71" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="47" t="s">
@@ -3571,13 +3570,13 @@
       <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="71" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="50">
         <v>1</v>
       </c>
       <c r="E10" s="49">
@@ -3715,14 +3714,14 @@
       <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="51">
-        <v>0.5</v>
+      <c r="D11" s="50">
+        <v>0.8</v>
       </c>
       <c r="E11" s="49">
         <v>45544</v>
@@ -3857,14 +3856,14 @@
     </row>
     <row r="12" spans="1:127" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="72" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="51">
-        <v>0.8</v>
+      <c r="D12" s="50">
+        <v>1</v>
       </c>
       <c r="E12" s="49">
         <v>45544</v>
@@ -3996,13 +3995,13 @@
     </row>
     <row r="13" spans="1:127" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="50">
         <v>1</v>
       </c>
       <c r="E13" s="49">
@@ -4140,10 +4139,10 @@
       <c r="B14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
       <c r="G14" s="35"/>
       <c r="H14" s="11" t="str">
         <f t="shared" si="75"/>
@@ -4271,13 +4270,13 @@
     </row>
     <row r="15" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="50">
         <v>1</v>
       </c>
       <c r="E15" s="49">
@@ -4410,13 +4409,13 @@
     </row>
     <row r="16" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="51">
+      <c r="D16" s="50">
         <v>1</v>
       </c>
       <c r="E16" s="49">
@@ -4552,13 +4551,13 @@
     </row>
     <row r="17" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="50">
         <v>1</v>
       </c>
       <c r="E17" s="49">
@@ -4694,13 +4693,13 @@
     </row>
     <row r="18" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="50">
         <v>1</v>
       </c>
       <c r="E18" s="49">
@@ -4836,14 +4835,14 @@
     </row>
     <row r="19" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="72" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="51">
-        <v>0.7</v>
+      <c r="D19" s="50">
+        <v>1</v>
       </c>
       <c r="E19" s="49">
         <v>45566</v>
@@ -4978,20 +4977,20 @@
     </row>
     <row r="20" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="51">
-        <v>0.1</v>
+      <c r="C20" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="50">
+        <v>0.7</v>
       </c>
       <c r="E20" s="49">
         <v>45566</v>
       </c>
       <c r="F20" s="49">
-        <v>45656</v>
+        <v>45646</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -5117,20 +5116,20 @@
     </row>
     <row r="21" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="51">
-        <v>0.1</v>
+      <c r="C21" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="50">
+        <v>0.7</v>
       </c>
       <c r="E21" s="49">
         <v>45566</v>
       </c>
       <c r="F21" s="49">
-        <v>45657</v>
+        <v>45646</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -5256,25 +5255,25 @@
     </row>
     <row r="22" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="51">
-        <v>0.1</v>
+      <c r="C22" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="50">
+        <v>0.7</v>
       </c>
       <c r="E22" s="49">
         <v>45566</v>
       </c>
       <c r="F22" s="49">
-        <v>45657</v>
+        <v>45646</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11">
         <f t="shared" si="75"/>
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
@@ -5398,20 +5397,20 @@
     </row>
     <row r="23" spans="1:127" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="51">
-        <v>0.1</v>
+      <c r="C23" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="50">
+        <v>0.7</v>
       </c>
       <c r="E23" s="49">
         <v>45566</v>
       </c>
       <c r="F23" s="49">
-        <v>45657</v>
+        <v>45646</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -5542,10 +5541,10 @@
       <c r="B24" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="59"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58"/>
       <c r="G24" s="39"/>
       <c r="H24" s="11" t="str">
         <f t="shared" si="75"/>
@@ -5679,15 +5678,19 @@
       <c r="C25" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="51">
-        <v>0</v>
-      </c>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
+      <c r="D25" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E25" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F25" s="49">
+        <v>45646</v>
+      </c>
       <c r="G25" s="11"/>
-      <c r="H25" s="11" t="str">
+      <c r="H25" s="11">
         <f t="shared" si="75"/>
-        <v/>
+        <v>81</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
@@ -5814,18 +5817,22 @@
       <c r="B26" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="51">
-        <v>0</v>
-      </c>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
+      <c r="D26" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E26" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F26" s="49">
+        <v>45646</v>
+      </c>
       <c r="G26" s="11"/>
-      <c r="H26" s="11" t="str">
+      <c r="H26" s="11">
         <f t="shared" si="75"/>
-        <v/>
+        <v>81</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
@@ -5952,18 +5959,22 @@
       <c r="B27" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="74" t="s">
+      <c r="C27" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="51">
-        <v>0</v>
-      </c>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
+      <c r="D27" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E27" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F27" s="49">
+        <v>45646</v>
+      </c>
       <c r="G27" s="11"/>
-      <c r="H27" s="11" t="str">
+      <c r="H27" s="11">
         <f t="shared" si="75"/>
-        <v/>
+        <v>81</v>
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
@@ -6090,18 +6101,22 @@
       <c r="B28" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="51">
-        <v>0</v>
-      </c>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
+      <c r="C28" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E28" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F28" s="49">
+        <v>45646</v>
+      </c>
       <c r="G28" s="11"/>
-      <c r="H28" s="11" t="str">
+      <c r="H28" s="11">
         <f t="shared" si="75"/>
-        <v/>
+        <v>81</v>
       </c>
       <c r="I28" s="16"/>
       <c r="J28" s="16"/>
@@ -6228,14 +6243,18 @@
       <c r="B29" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="51">
-        <v>0</v>
-      </c>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
+      <c r="D29" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E29" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F29" s="49">
+        <v>45646</v>
+      </c>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="16"/>
@@ -6366,11 +6385,15 @@
       <c r="C30" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="51">
-        <v>0</v>
-      </c>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
+      <c r="D30" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E30" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F30" s="49">
+        <v>45646</v>
+      </c>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="16"/>
@@ -6500,10 +6523,10 @@
       <c r="B31" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="60"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="63"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="37"/>
       <c r="H31" s="11" t="str">
         <f t="shared" si="75"/>
@@ -6634,16 +6657,22 @@
       <c r="B32" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="51">
-        <v>0</v>
-      </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
+      <c r="C32" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E32" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F32" s="49">
+        <v>45646</v>
+      </c>
       <c r="G32" s="11"/>
-      <c r="H32" s="11" t="str">
+      <c r="H32" s="11">
         <f t="shared" si="75"/>
-        <v/>
+        <v>81</v>
       </c>
       <c r="I32" s="16"/>
       <c r="J32" s="16"/>
@@ -6770,16 +6799,22 @@
       <c r="B33" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="51">
-        <v>0</v>
-      </c>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
+      <c r="C33" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E33" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F33" s="49">
+        <v>45646</v>
+      </c>
       <c r="G33" s="11"/>
-      <c r="H33" s="11" t="str">
+      <c r="H33" s="11">
         <f t="shared" si="75"/>
-        <v/>
+        <v>81</v>
       </c>
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
@@ -6906,10 +6941,10 @@
       <c r="B34" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="64"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="67"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="41"/>
       <c r="H34" s="11"/>
       <c r="I34" s="16"/>
@@ -7037,12 +7072,18 @@
       <c r="B35" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="51">
-        <v>0</v>
-      </c>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
+      <c r="C35" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E35" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F35" s="49">
+        <v>45646</v>
+      </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" s="16"/>
@@ -7170,12 +7211,18 @@
       <c r="B36" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="51">
-        <v>0</v>
-      </c>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
+      <c r="C36" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E36" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F36" s="49">
+        <v>45646</v>
+      </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="16"/>
@@ -7303,12 +7350,18 @@
       <c r="B37" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="50"/>
-      <c r="D37" s="51">
-        <v>0</v>
-      </c>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
+      <c r="C37" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E37" s="49">
+        <v>45566</v>
+      </c>
+      <c r="F37" s="49">
+        <v>45646</v>
+      </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="16"/>
@@ -7438,10 +7491,10 @@
       <c r="B38" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="68"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="71"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="70"/>
       <c r="G38" s="15"/>
       <c r="H38" s="15" t="str">
         <f t="shared" si="75"/>
@@ -7579,6 +7632,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="DJ4:DP4"/>
     <mergeCell ref="DQ4:DW4"/>
     <mergeCell ref="CV4:DB4"/>
@@ -7588,17 +7652,6 @@
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D8 D16:D38 D10:D14">
     <cfRule type="dataBar" priority="22">
@@ -7615,20 +7668,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:DW38">
-    <cfRule type="expression" dxfId="3" priority="41">
+    <cfRule type="expression" dxfId="2" priority="41">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:DW38">
-    <cfRule type="expression" dxfId="2" priority="35">
+    <cfRule type="expression" dxfId="1" priority="35">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="36" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>I$5=_xludf.TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8015,15 +8068,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -8041,6 +8085,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8065,14 +8118,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
@@ -8089,4 +8134,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>